<commit_message>
PROS-8677 - CCRU - CCRU KPI issues
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC Canteen - EDU.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC Canteen - EDU.xlsx
@@ -14,6 +14,7 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Canteen!$A$1:$AL$54</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">Canteen!$A$1:$AL$54</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Canteen!$A$1:$AL$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Canteen!$A$1:$AL$54</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="260">
   <si>
     <t xml:space="preserve">Sorting</t>
   </si>
@@ -539,9 +540,6 @@
   </si>
   <si>
     <t xml:space="preserve">Manufacture: TCCC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola, Dobriy, Rich</t>
   </si>
   <si>
     <t xml:space="preserve">Coca-Cola, Dobriy, Rich, Fuzetea, Bonaqua, SmartWater</t>
@@ -1210,47 +1208,47 @@
   </sheetPr>
   <dimension ref="1:56"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F55" activeCellId="0" sqref="F55"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="N38" activeCellId="0" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.502024291498"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="68.663967611336"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="70.9109311740891"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="40.7044534412955"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="69.3076923076923"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="71.4493927125506"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="41.0283400809717"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="2" width="9"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="13.1740890688259"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="2" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="132.825910931174"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="80.9838056680162"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="45.2024291497976"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="72.9271255060729"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="81.7327935222672"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="45.6315789473684"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="2" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="24.6356275303644"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="2" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="29" min="28" style="2" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="2" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="2" width="59.0242914979757"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="2" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="2" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="29" min="28" style="2" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="2" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="2" width="59.4493927125506"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="2" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="35" min="35" style="2" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="36" min="36" style="2" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="37" min="37" style="2" width="10.6032388663968"/>
@@ -37419,7 +37417,7 @@
       </c>
       <c r="O35" s="9"/>
       <c r="P35" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q35" s="9" t="s">
         <v>63</v>
@@ -37432,10 +37430,10 @@
       <c r="U35" s="9"/>
       <c r="V35" s="9"/>
       <c r="W35" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="X35" s="9" t="s">
         <v>163</v>
-      </c>
-      <c r="X35" s="9" t="s">
-        <v>164</v>
       </c>
       <c r="Y35" s="9"/>
       <c r="Z35" s="9"/>
@@ -38465,10 +38463,10 @@
         <v>157</v>
       </c>
       <c r="F36" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G36" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>60</v>
@@ -38487,7 +38485,7 @@
       </c>
       <c r="O36" s="9"/>
       <c r="P36" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q36" s="9" t="s">
         <v>63</v>
@@ -38500,10 +38498,10 @@
       <c r="U36" s="9"/>
       <c r="V36" s="9"/>
       <c r="W36" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="X36" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y36" s="9"/>
       <c r="Z36" s="9"/>
@@ -39530,16 +39528,16 @@
         <v>40</v>
       </c>
       <c r="E37" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="F37" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="G37" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="H37" s="9" t="s">
         <v>170</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>171</v>
       </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
@@ -39550,7 +39548,7 @@
       <c r="O37" s="13"/>
       <c r="P37" s="13"/>
       <c r="Q37" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="R37" s="9"/>
       <c r="S37" s="9"/>
@@ -39564,7 +39562,7 @@
       <c r="AA37" s="9"/>
       <c r="AB37" s="9"/>
       <c r="AC37" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AD37" s="11" t="n">
         <v>0.135</v>
@@ -39572,7 +39570,7 @@
       <c r="AE37" s="9"/>
       <c r="AF37" s="9"/>
       <c r="AG37" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AH37" s="9"/>
       <c r="AI37" s="9" t="n">
@@ -39582,7 +39580,7 @@
         <v>31</v>
       </c>
       <c r="AK37" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AL37" s="9" t="n">
         <v>311</v>
@@ -40588,16 +40586,16 @@
         <v>40</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F38" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="G38" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="H38" s="9" t="s">
         <v>177</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>178</v>
       </c>
       <c r="I38" s="9"/>
       <c r="J38" s="9" t="n">
@@ -40606,7 +40604,7 @@
       <c r="K38" s="9"/>
       <c r="L38" s="9"/>
       <c r="M38" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N38" s="13"/>
       <c r="O38" s="13"/>
@@ -40618,7 +40616,7 @@
       <c r="U38" s="9"/>
       <c r="V38" s="9"/>
       <c r="W38" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="X38" s="9"/>
       <c r="Y38" s="9"/>
@@ -40632,7 +40630,7 @@
       <c r="AE38" s="9"/>
       <c r="AF38" s="9"/>
       <c r="AG38" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AH38" s="9"/>
       <c r="AI38" s="9" t="n">
@@ -41646,16 +41644,16 @@
         <v>40</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F39" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="G39" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="G39" s="9" t="s">
+      <c r="H39" s="9" t="s">
         <v>183</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>184</v>
       </c>
       <c r="I39" s="9"/>
       <c r="J39" s="9" t="n">
@@ -41664,23 +41662,23 @@
       <c r="K39" s="9"/>
       <c r="L39" s="9"/>
       <c r="M39" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N39" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O39" s="13"/>
       <c r="P39" s="13"/>
       <c r="Q39" s="9"/>
       <c r="R39" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="S39" s="9"/>
       <c r="T39" s="9"/>
       <c r="U39" s="9"/>
       <c r="V39" s="9"/>
       <c r="W39" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="X39" s="9"/>
       <c r="Y39" s="9"/>
@@ -42706,16 +42704,16 @@
         <v>40</v>
       </c>
       <c r="E40" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="F40" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="G40" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="G40" s="9" t="s">
+      <c r="H40" s="9" t="s">
         <v>190</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>191</v>
       </c>
       <c r="I40" s="9"/>
       <c r="J40" s="9" t="n">
@@ -42725,13 +42723,13 @@
       <c r="L40" s="9"/>
       <c r="M40" s="9"/>
       <c r="N40" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O40" s="13"/>
       <c r="P40" s="13"/>
       <c r="Q40" s="9"/>
       <c r="R40" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="S40" s="9"/>
       <c r="T40" s="9"/>
@@ -42741,7 +42739,7 @@
         <v>65</v>
       </c>
       <c r="X40" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Y40" s="9"/>
       <c r="Z40" s="9"/>
@@ -42756,10 +42754,10 @@
       <c r="AE40" s="9"/>
       <c r="AF40" s="9"/>
       <c r="AG40" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AH40" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AI40" s="9" t="n">
         <v>2</v>
@@ -43772,16 +43770,16 @@
         <v>40</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F41" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="G41" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="H41" s="9" t="s">
         <v>196</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>197</v>
       </c>
       <c r="I41" s="9"/>
       <c r="J41" s="9" t="n">
@@ -43790,23 +43788,23 @@
       <c r="K41" s="9"/>
       <c r="L41" s="9"/>
       <c r="M41" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N41" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O41" s="13"/>
       <c r="P41" s="13"/>
       <c r="Q41" s="9"/>
       <c r="R41" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="S41" s="9"/>
       <c r="T41" s="9"/>
       <c r="U41" s="9"/>
       <c r="V41" s="9"/>
       <c r="W41" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="X41" s="9"/>
       <c r="Y41" s="9"/>
@@ -43814,7 +43812,7 @@
       <c r="AA41" s="9"/>
       <c r="AB41" s="9"/>
       <c r="AC41" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AD41" s="11" t="n">
         <v>0.045</v>
@@ -43822,10 +43820,10 @@
       <c r="AE41" s="9"/>
       <c r="AF41" s="9"/>
       <c r="AG41" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AH41" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AI41" s="9" t="n">
         <v>2</v>
@@ -44838,16 +44836,16 @@
         <v>40</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F42" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="G42" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="G42" s="9" t="s">
+      <c r="H42" s="9" t="s">
         <v>200</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>201</v>
       </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
@@ -44858,23 +44856,23 @@
         <v>15</v>
       </c>
       <c r="M42" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N42" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O42" s="13"/>
       <c r="P42" s="13"/>
       <c r="Q42" s="9"/>
       <c r="R42" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="S42" s="9"/>
       <c r="T42" s="9"/>
       <c r="U42" s="9"/>
       <c r="V42" s="9"/>
       <c r="W42" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="X42" s="9"/>
       <c r="Y42" s="9"/>
@@ -44882,7 +44880,7 @@
       <c r="AA42" s="9"/>
       <c r="AB42" s="9"/>
       <c r="AC42" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AD42" s="11" t="n">
         <v>0.045</v>
@@ -44890,10 +44888,10 @@
       <c r="AE42" s="9"/>
       <c r="AF42" s="9"/>
       <c r="AG42" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AH42" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AI42" s="9" t="n">
         <v>2</v>
@@ -45906,16 +45904,16 @@
         <v>40</v>
       </c>
       <c r="E43" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F43" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="G43" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="H43" s="9" t="s">
         <v>205</v>
-      </c>
-      <c r="H43" s="9" t="s">
-        <v>206</v>
       </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9" t="n">
@@ -45936,10 +45934,10 @@
       <c r="U43" s="9"/>
       <c r="V43" s="9"/>
       <c r="W43" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="X43" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y43" s="9"/>
       <c r="Z43" s="9"/>
@@ -45962,7 +45960,7 @@
         <v>37</v>
       </c>
       <c r="AK43" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AL43" s="20" t="n">
         <v>400</v>
@@ -46968,13 +46966,13 @@
         <v>40</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F44" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="G44" s="9" t="s">
         <v>209</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>210</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>60</v>
@@ -46986,16 +46984,16 @@
       <c r="K44" s="9"/>
       <c r="L44" s="9"/>
       <c r="M44" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="N44" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="N44" s="9" t="s">
+      <c r="O44" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="O44" s="9" t="s">
-        <v>213</v>
-      </c>
       <c r="P44" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Q44" s="9" t="s">
         <v>63</v>
@@ -47008,10 +47006,10 @@
       <c r="U44" s="9"/>
       <c r="V44" s="9"/>
       <c r="W44" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="X44" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y44" s="9"/>
       <c r="Z44" s="9"/>
@@ -48036,13 +48034,13 @@
         <v>40</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F45" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G45" s="9" t="s">
         <v>214</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>215</v>
       </c>
       <c r="H45" s="9" t="s">
         <v>60</v>
@@ -48054,13 +48052,13 @@
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>
       <c r="M45" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N45" s="9" t="n">
         <v>5000034</v>
       </c>
       <c r="O45" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P45" s="9"/>
       <c r="Q45" s="9" t="s">
@@ -48074,10 +48072,10 @@
       <c r="U45" s="9"/>
       <c r="V45" s="9"/>
       <c r="W45" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="X45" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y45" s="9"/>
       <c r="Z45" s="9"/>
@@ -48090,7 +48088,7 @@
       <c r="AE45" s="9"/>
       <c r="AF45" s="9"/>
       <c r="AG45" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AH45" s="9"/>
       <c r="AI45" s="9" t="n">
@@ -49104,16 +49102,16 @@
         <v>40</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F46" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="G46" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="G46" s="9" t="s">
-        <v>219</v>
-      </c>
       <c r="H46" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I46" s="9"/>
       <c r="J46" s="9" t="n">
@@ -49134,10 +49132,10 @@
       <c r="U46" s="9"/>
       <c r="V46" s="9"/>
       <c r="W46" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="X46" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y46" s="9"/>
       <c r="Z46" s="9"/>
@@ -49160,7 +49158,7 @@
         <v>40</v>
       </c>
       <c r="AK46" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AL46" s="9" t="n">
         <v>400</v>
@@ -50166,13 +50164,13 @@
         <v>40</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F47" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="G47" s="9" t="s">
         <v>221</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>222</v>
       </c>
       <c r="H47" s="9" t="s">
         <v>60</v>
@@ -50184,16 +50182,16 @@
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
       <c r="M47" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="N47" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="N47" s="9" t="s">
+      <c r="O47" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="P47" s="9" t="s">
         <v>224</v>
-      </c>
-      <c r="O47" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="P47" s="9" t="s">
-        <v>225</v>
       </c>
       <c r="Q47" s="9" t="s">
         <v>63</v>
@@ -50206,10 +50204,10 @@
       <c r="U47" s="9"/>
       <c r="V47" s="9"/>
       <c r="W47" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="X47" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y47" s="9"/>
       <c r="Z47" s="9"/>
@@ -51234,16 +51232,16 @@
         <v>40</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F48" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="G48" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="G48" s="9" t="s">
+      <c r="H48" s="9" t="s">
         <v>227</v>
-      </c>
-      <c r="H48" s="9" t="s">
-        <v>228</v>
       </c>
       <c r="I48" s="9"/>
       <c r="J48" s="9" t="n">
@@ -51252,13 +51250,13 @@
       <c r="K48" s="9"/>
       <c r="L48" s="9"/>
       <c r="M48" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N48" s="9" t="n">
         <v>5000034</v>
       </c>
       <c r="O48" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P48" s="9"/>
       <c r="Q48" s="9" t="s">
@@ -51272,10 +51270,10 @@
       <c r="U48" s="9"/>
       <c r="V48" s="9"/>
       <c r="W48" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="X48" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y48" s="9"/>
       <c r="Z48" s="9"/>
@@ -51288,7 +51286,7 @@
       <c r="AE48" s="9"/>
       <c r="AF48" s="9"/>
       <c r="AG48" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AH48" s="9"/>
       <c r="AI48" s="9" t="n">
@@ -52299,22 +52297,22 @@
         <v>39</v>
       </c>
       <c r="D49" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="F49" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="E49" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="F49" s="20" t="s">
+      <c r="G49" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="G49" s="20" t="s">
+      <c r="H49" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="H49" s="9" t="s">
+      <c r="I49" s="9" t="s">
         <v>232</v>
-      </c>
-      <c r="I49" s="9" t="s">
-        <v>233</v>
       </c>
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
@@ -52325,7 +52323,7 @@
       <c r="P49" s="9"/>
       <c r="Q49" s="9"/>
       <c r="R49" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="S49" s="9"/>
       <c r="T49" s="9"/>
@@ -53349,37 +53347,37 @@
         <v>39</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F50" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="G50" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="G50" s="9" t="s">
+      <c r="H50" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="H50" s="9" t="s">
+      <c r="I50" s="9" t="s">
         <v>237</v>
-      </c>
-      <c r="I50" s="9" t="s">
-        <v>238</v>
       </c>
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
       <c r="L50" s="9"/>
       <c r="M50" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="N50" s="14" t="s">
         <v>239</v>
-      </c>
-      <c r="N50" s="14" t="s">
-        <v>240</v>
       </c>
       <c r="O50" s="9"/>
       <c r="P50" s="9"/>
       <c r="Q50" s="9"/>
       <c r="R50" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="S50" s="9"/>
       <c r="T50" s="9"/>
@@ -54403,37 +54401,37 @@
         <v>39</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F51" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="G51" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="G51" s="9" t="s">
+      <c r="H51" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="H51" s="9" t="s">
+      <c r="I51" s="9" t="s">
         <v>237</v>
-      </c>
-      <c r="I51" s="9" t="s">
-        <v>238</v>
       </c>
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
       <c r="L51" s="9"/>
       <c r="M51" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N51" s="14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O51" s="9"/>
       <c r="P51" s="9"/>
       <c r="Q51" s="9"/>
       <c r="R51" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="S51" s="9"/>
       <c r="T51" s="9"/>
@@ -55457,37 +55455,37 @@
         <v>39</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E52" s="20" t="s">
         <v>157</v>
       </c>
       <c r="F52" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="G52" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="G52" s="20" t="s">
-        <v>243</v>
-      </c>
       <c r="H52" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="I52" s="9" t="s">
         <v>237</v>
-      </c>
-      <c r="I52" s="9" t="s">
-        <v>238</v>
       </c>
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
       <c r="L52" s="9"/>
       <c r="M52" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N52" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O52" s="9"/>
       <c r="P52" s="9"/>
       <c r="Q52" s="9"/>
       <c r="R52" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="S52" s="9"/>
       <c r="T52" s="9"/>
@@ -56511,37 +56509,37 @@
         <v>39</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E53" s="20" t="s">
         <v>157</v>
       </c>
       <c r="F53" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="G53" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="G53" s="20" t="s">
-        <v>243</v>
-      </c>
       <c r="H53" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="I53" s="9" t="s">
         <v>237</v>
-      </c>
-      <c r="I53" s="9" t="s">
-        <v>238</v>
       </c>
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
       <c r="L53" s="9"/>
       <c r="M53" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N53" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O53" s="9"/>
       <c r="P53" s="9"/>
       <c r="Q53" s="9"/>
       <c r="R53" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="S53" s="9"/>
       <c r="T53" s="9"/>
@@ -57565,37 +57563,37 @@
         <v>39</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E54" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="F54" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="F54" s="20" t="s">
+      <c r="G54" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="G54" s="20" t="s">
-        <v>248</v>
-      </c>
       <c r="H54" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="I54" s="9" t="s">
         <v>237</v>
-      </c>
-      <c r="I54" s="9" t="s">
-        <v>238</v>
       </c>
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
       <c r="L54" s="9"/>
       <c r="M54" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="N54" s="14" t="s">
         <v>249</v>
-      </c>
-      <c r="N54" s="14" t="s">
-        <v>250</v>
       </c>
       <c r="O54" s="9"/>
       <c r="P54" s="9"/>
       <c r="Q54" s="9"/>
       <c r="R54" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="S54" s="9"/>
       <c r="T54" s="9"/>
@@ -57618,7 +57616,7 @@
         <v>48</v>
       </c>
       <c r="AK54" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AL54" s="9"/>
       <c r="AM54" s="0"/>
@@ -58619,42 +58617,42 @@
         <v>39</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E55" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="F55" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="F55" s="21" t="s">
+      <c r="G55" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="G55" s="21" t="s">
+      <c r="H55" s="22" t="s">
         <v>254</v>
       </c>
-      <c r="H55" s="22" t="s">
-        <v>255</v>
-      </c>
       <c r="I55" s="22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J55" s="23"/>
       <c r="K55" s="23"/>
       <c r="L55" s="23"/>
       <c r="M55" s="8"/>
       <c r="N55" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O55" s="8"/>
       <c r="P55" s="8"/>
       <c r="Q55" s="8"/>
       <c r="R55" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="S55" s="8"/>
       <c r="T55" s="8"/>
       <c r="U55" s="8"/>
       <c r="V55" s="8"/>
       <c r="W55" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="X55" s="25"/>
       <c r="Y55" s="8"/>
@@ -59671,20 +59669,20 @@
         <v>39</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E56" s="27"/>
       <c r="F56" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="G56" s="27" t="s">
         <v>258</v>
       </c>
-      <c r="G56" s="27" t="s">
+      <c r="H56" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="I56" s="8" t="s">
         <v>259</v>
-      </c>
-      <c r="H56" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="I56" s="8" t="s">
-        <v>260</v>
       </c>
       <c r="J56" s="23"/>
       <c r="K56" s="23"/>
@@ -59695,7 +59693,7 @@
       <c r="P56" s="8"/>
       <c r="Q56" s="8"/>
       <c r="R56" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="S56" s="8"/>
       <c r="T56" s="8"/>

</xml_diff>

<commit_message>
PROS-9087 - CCRU - rename KPIs at POS
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC Canteen - EDU.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC Canteen - EDU.xlsx
@@ -15,6 +15,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">Canteen!$A$1:$AL$54</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Canteen!$A$1:$AL$54</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Canteen!$A$1:$AL$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Canteen!$A$1:$AL$54</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -219,7 +220,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Coca-Cola - 0.25L Slim/Coca-Cola - 0.33L Glass</t>
+    <t xml:space="preserve">Coca-Cola - 0.25L Slim/0.33L Glass</t>
   </si>
   <si>
     <t xml:space="preserve">Кока-Кола - 0.25л слим/Кока-Кола - 0.33л стекло</t>
@@ -249,7 +250,7 @@
     <t xml:space="preserve">BINARY</t>
   </si>
   <si>
-    <t xml:space="preserve">Coca-Cola Zero/Cherry - 0.25L /Coca-Cola Zero - 0.33L Glass</t>
+    <t xml:space="preserve">Coca-Cola Zero - 0.25L Slim/0.33L Glass/Coca-Cola Zero Cherry - 0.25L Slim</t>
   </si>
   <si>
     <t xml:space="preserve">Кока-Кола Зеро/Вишня - 0.25л слим/Кока-Кола Зеро - 0.33л стекло</t>
@@ -297,7 +298,7 @@
     <t xml:space="preserve">Спрайт - 0.5л</t>
   </si>
   <si>
-    <t xml:space="preserve">Coca-Cola Zero/Zero Cherry - 0.5L</t>
+    <t xml:space="preserve">Coca-Cola Zero/Coca-Cola Zero Cherry - 0.5L</t>
   </si>
   <si>
     <t xml:space="preserve">Кока-Кола Зеро/Вишня - 0.5л</t>
@@ -315,7 +316,7 @@
     <t xml:space="preserve">Фанта Апельсин - 0.5л</t>
   </si>
   <si>
-    <t xml:space="preserve">Fanta Citrus/Pear - 0.5L - 0.5L</t>
+    <t xml:space="preserve">Fanta Citrus - 0.5L/Fanta Pear - 0.5L</t>
   </si>
   <si>
     <t xml:space="preserve">Фанта Цитрус/Груша - 0.5л - 0.5л</t>
@@ -357,7 +358,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">BonAqua Still/Carb 0-33/0.5L SmartWater Still-0.6L</t>
+    <t xml:space="preserve">BonAqua Still/Carb - 0.5L/0.33L Glass/SmartWater Still - 0.6L</t>
   </si>
   <si>
     <t xml:space="preserve">БонАква Негаз/Газ-0.5л /Смарт вода-0.6л/БонАква Негаз/ Газ-0.33л стекло</t>
@@ -421,7 +422,7 @@
     <t xml:space="preserve">4607042430879, 5449000027450</t>
   </si>
   <si>
-    <t xml:space="preserve">Fuze Berry-Hibiscus/Lemon-Lemongrass - 0.5L</t>
+    <t xml:space="preserve">Fuze Berry-Hibiscus - 0.5L/Fuze Lemon-Lemongrass - 0.5L</t>
   </si>
   <si>
     <t xml:space="preserve">Фьюз Лесн.ягоды/Лимон - 0.5л</t>
@@ -433,7 +434,7 @@
     <t xml:space="preserve">5449000259455, 5449000235947, 5449000193124, 5449000189301</t>
   </si>
   <si>
-    <t xml:space="preserve">Fuze Green Strawberry-Raspberry/Peach-Rose/Green Citrus - 0.5L</t>
+    <t xml:space="preserve">Fuze Green Strawberry-Raspberry - 0.5L/Peach-Rose/Green Citrus - 0.5L</t>
   </si>
   <si>
     <t xml:space="preserve">Фьюз Зеленый Клубника/Персик/Зеленый Цитрус - 0.5л</t>
@@ -461,7 +462,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Dobriy - Apple -0.33L/Rich - Apple - 0.3L/0.2L Glass</t>
+    <t xml:space="preserve">Dobriy - Apple - 0.33L/Rich - Apple - 0.3L/0.2L Glass</t>
   </si>
   <si>
     <t xml:space="preserve">Добрый - Яблоко - 0.33л/Рич - Яблоко - 0.3л/0.2л стекло</t>
@@ -485,7 +486,7 @@
     <t xml:space="preserve">Палпи - Манго Ананас - 0.45л</t>
   </si>
   <si>
-    <t xml:space="preserve">Dobriy - Multifruit - 0.33L/ Rich - Orange - 0.2L Glass/0.3L </t>
+    <t xml:space="preserve">Dobriy - Multifruit - 0.33L/Rich - Orange - 0.2L Glass/0.3L </t>
   </si>
   <si>
     <t xml:space="preserve">Добрый-Мультифрут-0.33л/ Рич- Апельсин-0.2л стекло/ 0.3л </t>
@@ -497,7 +498,7 @@
     <t xml:space="preserve">4607174579286, 4650075420362, 4650075421024</t>
   </si>
   <si>
-    <t xml:space="preserve">Dobriy-Tomato-0.33L /Rich-Cherry-0.2L Glass/0.3L </t>
+    <t xml:space="preserve">Dobriy - Tomato - 0.33L/Rich - Cherry - 0.2L Glass/0.3L </t>
   </si>
   <si>
     <t xml:space="preserve">Добрый-Томат-0.33л/ Рич-Вишня-0.2л стекло/0.3л </t>
@@ -518,7 +519,7 @@
     <t xml:space="preserve">Pulpy - Tropical - 0.45L, Pulpy - Guava - 0.45L, Pulpy - Watermelon Strawberry - 0.45L</t>
   </si>
   <si>
-    <t xml:space="preserve">Dobriy-Peach-Apple/Orange-0.33L/Rich-Peach/Pineapple/Grapefruit/Tomato-0.2L Glass</t>
+    <t xml:space="preserve">Dobriy - Peach-Apple/Orange - 0.33L/Rich - Peach/Pineapple/Grapefruit/Tomato - 0.2L Glass</t>
   </si>
   <si>
     <t xml:space="preserve">Добрый-Персик/Апельсин-0.33л /Рич-Персик/Ананас/Грейпфру/Томат-0.2л стекло</t>
@@ -1208,47 +1209,47 @@
   </sheetPr>
   <dimension ref="1:56"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="N38" activeCellId="0" sqref="N38"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F1" activeCellId="0" sqref="F:F"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1781376518219"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="69.3076923076923"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="71.4493927125506"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="41.0283400809717"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="69.9473684210526"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="72.0890688259109"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="41.3481781376518"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="2" width="9"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="2" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="72.9271255060729"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="81.7327935222672"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="45.6315789473684"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="73.4817813765182"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="82.4817813765182"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="46.0607287449393"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="12.4251012145749"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="2" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="2" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="29" min="28" style="2" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="2" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="2" width="59.4493927125506"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="2" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="2" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="29" min="28" style="2" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="2" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="2" width="59.9878542510121"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="2" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="35" min="35" style="2" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="36" min="36" style="2" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="37" min="37" style="2" width="10.6032388663968"/>
@@ -58606,7 +58607,7 @@
       <c r="AMI54" s="0"/>
       <c r="AMJ54" s="0"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="8" t="n">
         <v>51</v>
       </c>
@@ -59658,7 +59659,7 @@
       <c r="AMI55" s="0"/>
       <c r="AMJ55" s="0"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="8" t="n">
         <v>401</v>
       </c>

</xml_diff>

<commit_message>
SD-113018 - CCRU - POS IC KPI templates update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC Canteen - EDU.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC Canteen - EDU.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuri\Downloads\CCRU new KPI\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My folder\RED\POS 2019\POS_2019-12-04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FFD94BA-27E4-46D1-B79A-FEA8977C8D80}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C2B602-946C-4657-BB72-B0F234477796}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="611" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="611" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Canteen" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,14 @@
     <definedName name="_FilterDatabase_0_0_0_0_0_0" localSheetId="0">Canteen!$A$1:$AN$1</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0" localSheetId="0">Canteen!$A$1:$AN$1</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -858,9 +864,6 @@
     <t>Integer</t>
   </si>
   <si>
-    <t>Bufet line, SS_Bufet line</t>
-  </si>
-  <si>
     <t>Panoramic Photo, SS_Panoramic Photo</t>
   </si>
   <si>
@@ -886,6 +889,9 @@
   </si>
   <si>
     <t>Juices</t>
+  </si>
+  <si>
+    <t>Bufet line, SS_Bufet line, Promo SSD Display IC</t>
   </si>
 </sst>
 </file>
@@ -916,7 +922,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -927,6 +933,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -972,7 +984,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1015,6 +1027,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1401,56 +1416,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMM57"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J62" sqref="J62"/>
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="Q1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z42" sqref="Z42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="6"/>
-    <col min="2" max="2" width="13.28515625" style="6"/>
-    <col min="3" max="3" width="15.5703125" style="6"/>
-    <col min="4" max="4" width="13.28515625" style="6"/>
-    <col min="5" max="5" width="16.28515625" style="6"/>
-    <col min="6" max="6" width="44.28515625" style="6"/>
-    <col min="7" max="7" width="90.140625" style="6"/>
-    <col min="8" max="8" width="48.85546875" style="6"/>
+    <col min="1" max="1" width="13.109375" style="6"/>
+    <col min="2" max="2" width="13.33203125" style="6"/>
+    <col min="3" max="3" width="15.5546875" style="6"/>
+    <col min="4" max="4" width="13.33203125" style="6"/>
+    <col min="5" max="5" width="16.33203125" style="6"/>
+    <col min="6" max="6" width="44.33203125" style="6"/>
+    <col min="7" max="7" width="90.109375" style="6"/>
+    <col min="8" max="8" width="48.88671875" style="6"/>
     <col min="9" max="9" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" style="6"/>
-    <col min="12" max="12" width="11.28515625" style="6"/>
-    <col min="13" max="14" width="16.28515625" style="6"/>
-    <col min="15" max="15" width="33.5703125" style="6"/>
-    <col min="16" max="16" width="33.5703125" style="12"/>
-    <col min="17" max="17" width="22.5703125" style="6"/>
-    <col min="18" max="18" width="55.85546875" style="6"/>
-    <col min="19" max="19" width="21.28515625" style="6"/>
+    <col min="10" max="10" width="25.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" style="6"/>
+    <col min="12" max="12" width="11.33203125" style="6"/>
+    <col min="13" max="14" width="16.33203125" style="6"/>
+    <col min="15" max="15" width="33.5546875" style="6"/>
+    <col min="16" max="16" width="33.5546875" style="12"/>
+    <col min="17" max="17" width="22.5546875" style="6"/>
+    <col min="18" max="18" width="55.88671875" style="6"/>
+    <col min="19" max="19" width="21.33203125" style="6"/>
     <col min="20" max="20" width="14" style="6"/>
-    <col min="21" max="21" width="9.140625" style="6"/>
-    <col min="22" max="22" width="16.28515625" style="6"/>
-    <col min="23" max="23" width="20.7109375" style="6"/>
-    <col min="24" max="25" width="25.7109375" style="6"/>
-    <col min="26" max="26" width="26.5703125" style="6"/>
-    <col min="27" max="27" width="23.140625" style="6"/>
-    <col min="28" max="28" width="29.42578125" style="6"/>
-    <col min="29" max="29" width="29.7109375" style="6"/>
-    <col min="30" max="30" width="19.42578125" style="6"/>
-    <col min="31" max="31" width="18.85546875" style="6"/>
-    <col min="32" max="32" width="16.28515625" style="13"/>
-    <col min="33" max="33" width="15.85546875" style="6"/>
-    <col min="34" max="34" width="16.140625" style="6"/>
-    <col min="35" max="35" width="73.7109375" style="6"/>
-    <col min="36" max="36" width="25.7109375" style="6"/>
-    <col min="37" max="37" width="10.28515625" style="6"/>
-    <col min="38" max="38" width="10.7109375" style="6"/>
-    <col min="39" max="39" width="18.85546875" style="12"/>
-    <col min="40" max="40" width="11.42578125" style="6"/>
-    <col min="41" max="1027" width="9.140625" style="6" customWidth="1"/>
-    <col min="1028" max="16384" width="8.85546875" style="7"/>
+    <col min="21" max="21" width="9.109375" style="6"/>
+    <col min="22" max="22" width="16.33203125" style="6"/>
+    <col min="23" max="23" width="20.6640625" style="6"/>
+    <col min="24" max="25" width="25.6640625" style="6"/>
+    <col min="26" max="26" width="26.5546875" style="6"/>
+    <col min="27" max="27" width="23.109375" style="6"/>
+    <col min="28" max="28" width="29.44140625" style="6"/>
+    <col min="29" max="29" width="29.6640625" style="6"/>
+    <col min="30" max="30" width="19.44140625" style="6"/>
+    <col min="31" max="31" width="18.88671875" style="6"/>
+    <col min="32" max="32" width="16.33203125" style="13"/>
+    <col min="33" max="33" width="15.88671875" style="6"/>
+    <col min="34" max="34" width="16.109375" style="6"/>
+    <col min="35" max="35" width="73.6640625" style="6"/>
+    <col min="36" max="36" width="25.6640625" style="6"/>
+    <col min="37" max="37" width="10.33203125" style="6"/>
+    <col min="38" max="38" width="10.6640625" style="6"/>
+    <col min="39" max="39" width="18.88671875" style="12"/>
+    <col min="40" max="40" width="11.44140625" style="6"/>
+    <col min="41" max="1027" width="9.109375" style="6" customWidth="1"/>
+    <col min="1028" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1476,10 +1491,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>263</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>264</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -1572,7 +1587,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1632,7 +1647,7 @@
       <c r="AM2" s="4"/>
       <c r="AN2" s="3"/>
     </row>
-    <row r="3" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>6</v>
       </c>
@@ -1661,7 +1676,7 @@
         <v>41</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -1704,7 +1719,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>7</v>
       </c>
@@ -1760,7 +1775,7 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB4" s="3"/>
       <c r="AC4" s="3"/>
@@ -1786,7 +1801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>7</v>
       </c>
@@ -1842,7 +1857,7 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB5" s="3"/>
       <c r="AC5" s="3"/>
@@ -1868,7 +1883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>9</v>
       </c>
@@ -1924,7 +1939,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
@@ -1950,7 +1965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>9</v>
       </c>
@@ -2006,7 +2021,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
       <c r="AA7" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
@@ -2032,7 +2047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>9</v>
       </c>
@@ -2088,7 +2103,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
@@ -2114,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>9</v>
       </c>
@@ -2170,7 +2185,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
@@ -2196,7 +2211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2252,7 +2267,7 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
@@ -2278,7 +2293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -2334,7 +2349,7 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
       <c r="AA11" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
@@ -2360,7 +2375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>15</v>
       </c>
@@ -2416,7 +2431,7 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
       <c r="AA12" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
@@ -2440,7 +2455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -2496,7 +2511,7 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
       <c r="AA13" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
@@ -2522,7 +2537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>9</v>
       </c>
@@ -2578,7 +2593,7 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
       <c r="AA14" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB14" s="3"/>
       <c r="AC14" s="3"/>
@@ -2604,7 +2619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>17</v>
       </c>
@@ -2633,7 +2648,7 @@
         <v>41</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -2676,7 +2691,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>18</v>
       </c>
@@ -2732,7 +2747,7 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
       <c r="AA16" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
@@ -2758,7 +2773,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>19</v>
       </c>
@@ -2814,7 +2829,7 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
       <c r="AA17" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB17" s="3"/>
       <c r="AC17" s="3"/>
@@ -2840,7 +2855,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>20</v>
       </c>
@@ -2896,7 +2911,7 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
       <c r="AA18" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB18" s="3"/>
       <c r="AC18" s="3"/>
@@ -2922,7 +2937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>21</v>
       </c>
@@ -2951,7 +2966,7 @@
         <v>41</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -2994,7 +3009,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="20" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>23</v>
       </c>
@@ -3050,7 +3065,7 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
       <c r="AA20" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB20" s="3"/>
       <c r="AC20" s="3"/>
@@ -3076,7 +3091,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>23</v>
       </c>
@@ -3132,7 +3147,7 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
       <c r="AA21" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB21" s="3"/>
       <c r="AC21" s="3"/>
@@ -3158,7 +3173,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>25</v>
       </c>
@@ -3214,7 +3229,7 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
       <c r="AA22" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB22" s="3"/>
       <c r="AC22" s="3"/>
@@ -3240,7 +3255,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>23</v>
       </c>
@@ -3296,7 +3311,7 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
       <c r="AA23" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB23" s="3"/>
       <c r="AC23" s="3"/>
@@ -3322,7 +3337,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>26</v>
       </c>
@@ -3351,7 +3366,7 @@
         <v>41</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
@@ -3394,7 +3409,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="25" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>27</v>
       </c>
@@ -3450,7 +3465,7 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
       <c r="AA25" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB25" s="3"/>
       <c r="AC25" s="3"/>
@@ -3476,7 +3491,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>28</v>
       </c>
@@ -3532,7 +3547,7 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
       <c r="AA26" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB26" s="3"/>
       <c r="AC26" s="3"/>
@@ -3558,7 +3573,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>28</v>
       </c>
@@ -3614,7 +3629,7 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
       <c r="AA27" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB27" s="3"/>
       <c r="AC27" s="3"/>
@@ -3640,7 +3655,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>29</v>
       </c>
@@ -3696,7 +3711,7 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
       <c r="AA28" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB28" s="3"/>
       <c r="AC28" s="3"/>
@@ -3722,7 +3737,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>30</v>
       </c>
@@ -3778,7 +3793,7 @@
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
       <c r="AA29" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB29" s="3"/>
       <c r="AC29" s="3"/>
@@ -3804,7 +3819,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>31</v>
       </c>
@@ -3860,7 +3875,7 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
       <c r="AA30" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB30" s="3"/>
       <c r="AC30" s="3"/>
@@ -3886,7 +3901,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>32</v>
       </c>
@@ -3942,7 +3957,7 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
       <c r="AA31" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
@@ -3968,7 +3983,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>2</v>
       </c>
@@ -4028,7 +4043,7 @@
       <c r="AM32" s="4"/>
       <c r="AN32" s="3"/>
     </row>
-    <row r="33" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>3</v>
       </c>
@@ -4090,7 +4105,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="34" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>36</v>
       </c>
@@ -4164,7 +4179,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="35" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>37</v>
       </c>
@@ -4238,7 +4253,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>38</v>
       </c>
@@ -4314,7 +4329,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>4</v>
       </c>
@@ -4378,7 +4393,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="38" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>39</v>
       </c>
@@ -4429,7 +4444,7 @@
         <v>55</v>
       </c>
       <c r="Z38" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AA38" s="3"/>
       <c r="AB38" s="3"/>
@@ -4460,7 +4475,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="39" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>40</v>
       </c>
@@ -4542,7 +4557,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="40" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>41</v>
       </c>
@@ -4626,7 +4641,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="41" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>5</v>
       </c>
@@ -4688,7 +4703,7 @@
       </c>
       <c r="AN41" s="3"/>
     </row>
-    <row r="42" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>34</v>
       </c>
@@ -4744,8 +4759,8 @@
       <c r="Y42" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="Z42" s="3" t="s">
-        <v>259</v>
+      <c r="Z42" s="16" t="s">
+        <v>268</v>
       </c>
       <c r="AA42" s="3"/>
       <c r="AB42" s="3"/>
@@ -4772,7 +4787,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>36</v>
       </c>
@@ -4821,7 +4836,7 @@
         <v>199</v>
       </c>
       <c r="Z43" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AA43" s="3"/>
       <c r="AB43" s="3"/>
@@ -4850,7 +4865,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="44" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>42</v>
       </c>
@@ -4899,7 +4914,7 @@
         <v>199</v>
       </c>
       <c r="Z44" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AA44" s="3"/>
       <c r="AB44" s="3"/>
@@ -4926,7 +4941,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="45" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>43</v>
       </c>
@@ -4985,7 +5000,7 @@
         <v>199</v>
       </c>
       <c r="Z45" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AA45" s="3"/>
       <c r="AB45" s="3"/>
@@ -5010,7 +5025,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>44</v>
       </c>
@@ -5067,7 +5082,7 @@
         <v>199</v>
       </c>
       <c r="Z46" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AA46" s="3"/>
       <c r="AB46" s="3"/>
@@ -5094,7 +5109,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>45</v>
       </c>
@@ -5143,7 +5158,7 @@
         <v>199</v>
       </c>
       <c r="Z47" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AA47" s="3"/>
       <c r="AB47" s="3"/>
@@ -5170,7 +5185,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="48" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>46</v>
       </c>
@@ -5227,7 +5242,7 @@
         <v>199</v>
       </c>
       <c r="Z48" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AA48" s="3"/>
       <c r="AB48" s="3"/>
@@ -5252,7 +5267,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>47</v>
       </c>
@@ -5309,7 +5324,7 @@
         <v>199</v>
       </c>
       <c r="Z49" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AA49" s="3"/>
       <c r="AB49" s="3"/>
@@ -5336,7 +5351,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>48</v>
       </c>
@@ -5402,7 +5417,7 @@
       </c>
       <c r="AN50" s="3"/>
     </row>
-    <row r="51" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>49</v>
       </c>
@@ -5472,7 +5487,7 @@
       </c>
       <c r="AN51" s="3"/>
     </row>
-    <row r="52" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>50</v>
       </c>
@@ -5542,7 +5557,7 @@
       </c>
       <c r="AN52" s="3"/>
     </row>
-    <row r="53" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>51</v>
       </c>
@@ -5612,7 +5627,7 @@
       </c>
       <c r="AN53" s="3"/>
     </row>
-    <row r="54" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>52</v>
       </c>
@@ -5682,7 +5697,7 @@
       </c>
       <c r="AN54" s="3"/>
     </row>
-    <row r="55" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>53</v>
       </c>
@@ -5752,7 +5767,7 @@
       </c>
       <c r="AN55" s="3"/>
     </row>
-    <row r="56" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>54</v>
       </c>
@@ -5820,7 +5835,7 @@
       <c r="AM56" s="4"/>
       <c r="AN56" s="3"/>
     </row>
-    <row r="57" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:40" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>55</v>
       </c>

</xml_diff>